<commit_message>
fixing Empty Row Excel
</commit_message>
<xml_diff>
--- a/Excel/Book1.xlsx
+++ b/Excel/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Learn\Selenium\ConsoleApp1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0918CA2B-CCD3-4030-94B9-F409FE5B0580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AAC151-F3B6-477B-9E7D-661709CBBB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{76C7E416-40A7-4E60-9E0E-E2D2600FABD6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>RUN</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>asd</t>
-  </si>
-  <si>
-    <t>RUN_TEST</t>
   </si>
   <si>
     <t>Password123</t>
@@ -412,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A6E01B-996C-47BC-954A-729E52BF7764}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +424,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -441,10 +438,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,10 +449,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -466,7 +463,18 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>